<commit_message>
commit some things from windows
</commit_message>
<xml_diff>
--- a/分析結果.xlsx
+++ b/分析結果.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="725" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="Lexrank" sheetId="3" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="syria" sheetId="11" r:id="rId11"/>
     <sheet name="Crimea" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="70">
   <si>
     <t>GROUP1</t>
   </si>
@@ -211,12 +211,58 @@
     <t>LexRank</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Brexit</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>Missile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Catalan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crimea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crimea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gravitational</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gravitational</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewol</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syria</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>turkish</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -228,6 +274,13 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -258,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -267,6 +320,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -2292,11 +2347,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="609157896"/>
-        <c:axId val="609156720"/>
+        <c:axId val="417294272"/>
+        <c:axId val="417293096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="609157896"/>
+        <c:axId val="417294272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2339,7 +2394,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609156720"/>
+        <c:crossAx val="417293096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2347,7 +2402,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="609156720"/>
+        <c:axId val="417293096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2398,7 +2453,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609157896"/>
+        <c:crossAx val="417294272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4487,11 +4542,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="677045032"/>
-        <c:axId val="677033272"/>
+        <c:axId val="417295448"/>
+        <c:axId val="419202184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="677045032"/>
+        <c:axId val="417295448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4534,7 +4589,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677033272"/>
+        <c:crossAx val="419202184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4542,7 +4597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="677033272"/>
+        <c:axId val="419202184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4593,7 +4648,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677045032"/>
+        <c:crossAx val="417295448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6682,11 +6737,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="600446072"/>
-        <c:axId val="600446464"/>
+        <c:axId val="419198656"/>
+        <c:axId val="419199048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="600446072"/>
+        <c:axId val="419198656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6729,7 +6784,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600446464"/>
+        <c:crossAx val="419199048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6737,7 +6792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="600446464"/>
+        <c:axId val="419199048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6788,7 +6843,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600446072"/>
+        <c:crossAx val="419198656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8875,11 +8930,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="604513784"/>
-        <c:axId val="604512216"/>
+        <c:axId val="419201400"/>
+        <c:axId val="419200224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="604513784"/>
+        <c:axId val="419201400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8922,7 +8977,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="604512216"/>
+        <c:crossAx val="419200224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8930,7 +8985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="604512216"/>
+        <c:axId val="419200224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8981,7 +9036,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="604513784"/>
+        <c:crossAx val="419201400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11068,11 +11123,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="600448816"/>
-        <c:axId val="600447248"/>
+        <c:axId val="419202576"/>
+        <c:axId val="419203360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="600448816"/>
+        <c:axId val="419202576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11115,7 +11170,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600447248"/>
+        <c:crossAx val="419203360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11123,7 +11178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="600447248"/>
+        <c:axId val="419203360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11174,7 +11229,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600448816"/>
+        <c:crossAx val="419202576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13261,11 +13316,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="674966640"/>
-        <c:axId val="674965464"/>
+        <c:axId val="419201792"/>
+        <c:axId val="419204928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="674966640"/>
+        <c:axId val="419201792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13308,7 +13363,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="674965464"/>
+        <c:crossAx val="419204928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13316,7 +13371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="674965464"/>
+        <c:axId val="419204928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13367,7 +13422,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="674966640"/>
+        <c:crossAx val="419201792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15178,11 +15233,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="600752472"/>
-        <c:axId val="600749728"/>
+        <c:axId val="419202968"/>
+        <c:axId val="419204144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="600752472"/>
+        <c:axId val="419202968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15225,7 +15280,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600749728"/>
+        <c:crossAx val="419204144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15233,7 +15288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="600749728"/>
+        <c:axId val="419204144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15284,7 +15339,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600752472"/>
+        <c:crossAx val="419202968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17371,11 +17426,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="600753256"/>
-        <c:axId val="600751296"/>
+        <c:axId val="419205320"/>
+        <c:axId val="419197872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="600753256"/>
+        <c:axId val="419205320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17418,7 +17473,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600751296"/>
+        <c:crossAx val="419197872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17426,7 +17481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="600751296"/>
+        <c:axId val="419197872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17477,7 +17532,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600753256"/>
+        <c:crossAx val="419205320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19564,11 +19619,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="609159072"/>
-        <c:axId val="609159856"/>
+        <c:axId val="420305224"/>
+        <c:axId val="420300912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="609159072"/>
+        <c:axId val="420305224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19611,7 +19666,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609159856"/>
+        <c:crossAx val="420300912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19619,7 +19674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="609159856"/>
+        <c:axId val="420300912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19670,7 +19725,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609159072"/>
+        <c:crossAx val="420305224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24759,16 +24814,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25357,15 +25412,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -25384,8 +25448,20 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -25404,8 +25480,26 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(C2,C4,C5,C6,C7,C14)</f>
+        <v>9.0808333333333338E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>6.3159999999999994E-2</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(C8,C9,C16)</f>
+        <v>0.10300666666666668</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(C10,C11)</f>
+        <v>4.292E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -25424,8 +25518,11 @@
       <c r="F3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -25444,8 +25541,11 @@
       <c r="F4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -25464,8 +25564,11 @@
       <c r="F5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -25484,8 +25587,11 @@
       <c r="F6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -25504,8 +25610,11 @@
       <c r="F7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -25524,8 +25633,11 @@
       <c r="F8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -25544,8 +25656,11 @@
       <c r="F9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -25564,8 +25679,11 @@
       <c r="F10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -25584,8 +25702,11 @@
       <c r="F11" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -25604,8 +25725,11 @@
       <c r="F12" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -25624,8 +25748,11 @@
       <c r="F13" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -25644,8 +25771,11 @@
       <c r="F14" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -25664,8 +25794,11 @@
       <c r="F15" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -25684,8 +25817,11 @@
       <c r="F16" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -25704,8 +25840,11 @@
       <c r="F17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -25724,8 +25863,11 @@
       <c r="F18" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -25744,8 +25886,11 @@
       <c r="F19" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -25763,6 +25908,9 @@
       </c>
       <c r="F20" s="1">
         <v>19</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -29321,8 +29469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" activeCellId="3" sqref="A1:A1048576 C1:C1048576 E1:E1048576 G1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -43026,14 +43174,15 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.36328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="12" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -49677,7 +49826,7 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -52892,7 +53041,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>

</xml_diff>